<commit_message>
Added default values columns for action setpoints.
</commit_message>
<xml_diff>
--- a/MySQL/configuration/fases_etapas.xlsx
+++ b/MySQL/configuration/fases_etapas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\UNIOVI\Master\IntegracionDeSistemas\TrabajoIntegracion\DockerIntegracion\MySQL\configuration\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A002020C-505A-49A7-B8B9-57E47D30D727}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C6977B3-09B8-4A9E-B214-36FE9760C3B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="7">
   <si>
     <t>id_fases_etapas</t>
   </si>
@@ -40,6 +40,12 @@
   </si>
   <si>
     <t>NULL</t>
+  </si>
+  <si>
+    <t>tipo_setpoint</t>
+  </si>
+  <si>
+    <t>valor_por_defecto_setpoint</t>
   </si>
 </sst>
 </file>
@@ -357,9 +363,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -367,9 +375,11 @@
     <col min="2" max="2" width="22" customWidth="1"/>
     <col min="3" max="3" width="21.21875" customWidth="1"/>
     <col min="4" max="4" width="21" customWidth="1"/>
+    <col min="5" max="5" width="17.77734375" customWidth="1"/>
+    <col min="6" max="6" width="23.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -382,8 +392,14 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
+      <c r="E1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -396,8 +412,14 @@
       <c r="D2" t="s">
         <v>4</v>
       </c>
+      <c r="E2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -410,8 +432,14 @@
       <c r="D3" t="s">
         <v>4</v>
       </c>
+      <c r="E3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -424,8 +452,14 @@
       <c r="D4" t="s">
         <v>4</v>
       </c>
+      <c r="E4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F4" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -436,6 +470,12 @@
         <v>3</v>
       </c>
       <c r="D5" t="s">
+        <v>4</v>
+      </c>
+      <c r="E5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F5" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>